<commit_message>
Implement clean industrial heat PTC policy (#322) (commit #3ef8208; 8/16/24)
</commit_message>
<xml_diff>
--- a/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
+++ b/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
@@ -1,27 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\web-app\BpTPEU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\web-app\BpTPEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{607ADCF9-16FE-4C87-95BD-6DD379138134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="14100"/>
+    <workbookView xWindow="57645" yWindow="2865" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BpTPEU-large" sheetId="2" r:id="rId2"/>
-    <sheet name="BpTPEU-small" sheetId="3" r:id="rId3"/>
+    <sheet name="BpTPEU-medium" sheetId="4" r:id="rId3"/>
+    <sheet name="BpTPEU-small" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Source:</t>
   </si>
@@ -54,12 +69,21 @@
   </si>
   <si>
     <t>BpTPEU BTU per Small Primary Energy Unit</t>
+  </si>
+  <si>
+    <t>BpTPEU BTU per Medium Primary Energy Unit</t>
+  </si>
+  <si>
+    <t>The medium primary energy output unit (used in the clean heat PTC policy) is: million BTU</t>
+  </si>
+  <si>
+    <t>medium primary energy output unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,14 +121,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -123,9 +146,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,9 +186,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,7 +223,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,7 +258,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,51 +431,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -463,7 +496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -471,17 +504,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -490,10 +523,10 @@
         <v>1000000000000000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
     </row>
   </sheetData>
@@ -502,7 +535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE14133-6F5B-4EE1-87AA-D9E510E794AA}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -510,29 +543,68 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <f>10^6</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
         <f>10^3</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subscript the industrial clean heat PTC policy by industrial heating process to allow for higher PTC rates for higher-temperature processes (#322) (commit #28c10fa; 8/16/24)
</commit_message>
<xml_diff>
--- a/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
+++ b/InputData/web-app/BpTPEU/BTU per Total Primary Energy Unit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\web-app\BpTPEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{607ADCF9-16FE-4C87-95BD-6DD379138134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D8FF91-0AC3-4137-91C4-6C89F0096FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57645" yWindow="2865" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57645" yWindow="2865" windowWidth="21600" windowHeight="12525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -539,9 +539,11 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -561,12 +563,6 @@
         <f>10^6</f>
         <v>1000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>